<commit_message>
Disabled window handler test cases
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/furnitureData.xlsx
+++ b/src/test/java/testdata/furnitureData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>MenuFromHome</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>79584585</t>
+  </si>
+  <si>
+    <t>70982197</t>
   </si>
 </sst>
 </file>
@@ -545,7 +548,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>